<commit_message>
Re-type Mislevy & Wu (1988) using LaTeX
</commit_message>
<xml_diff>
--- a/Administration/Training component.xlsx
+++ b/Administration/Training component.xlsx
@@ -1,26 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\Administration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7153F977-832A-449F-92B2-F5ABD70DC3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F743E1A-9390-49FB-AAFF-E561271D195C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="5460" windowWidth="17070" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="6105" windowWidth="17070" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Year</t>
   </si>
@@ -127,13 +136,16 @@
     <t>Vår</t>
   </si>
   <si>
-    <t>Enorlled</t>
-  </si>
-  <si>
     <t>Require confirmation</t>
   </si>
   <si>
     <t>Standard enrollment</t>
+  </si>
+  <si>
+    <t>Johan's latent variable model</t>
+  </si>
+  <si>
+    <t>Under construction</t>
   </si>
 </sst>
 </file>
@@ -248,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -326,6 +338,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -549,7 +570,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -615,8 +636,8 @@
         <f>F2</f>
         <v>3</v>
       </c>
-      <c r="H2" s="25" t="s">
-        <v>35</v>
+      <c r="H2" s="24" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -674,7 +695,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>28</v>
@@ -683,15 +704,21 @@
     <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="21"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="16">
+        <v>6</v>
+      </c>
       <c r="G6" s="21">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="17"/>
+        <v>15</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="27"/>
     </row>
     <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
@@ -714,10 +741,10 @@
       </c>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -726,7 +753,7 @@
       <c r="D8" s="3"/>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -735,7 +762,7 @@
       <c r="D9" s="3"/>
       <c r="G9" s="5">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -744,7 +771,7 @@
       <c r="D10" s="3"/>
       <c r="G10" s="5">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -753,7 +780,7 @@
       <c r="D11" s="3"/>
       <c r="G11" s="5">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -764,7 +791,7 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H12" s="21"/>
       <c r="I12" s="17"/>
@@ -790,10 +817,10 @@
       </c>
       <c r="G13" s="5">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>29</v>
@@ -805,7 +832,7 @@
       <c r="D14" s="3"/>
       <c r="G14" s="5">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -814,7 +841,7 @@
       <c r="D15" s="3"/>
       <c r="G15" s="5">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -823,7 +850,7 @@
       <c r="D16" s="3"/>
       <c r="G16" s="5">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -832,7 +859,7 @@
       <c r="D17" s="3"/>
       <c r="G17" s="5">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -843,7 +870,7 @@
       <c r="F18" s="21"/>
       <c r="G18" s="21">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H18" s="21"/>
       <c r="I18" s="17"/>
@@ -869,10 +896,10 @@
       </c>
       <c r="G19" s="5">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -881,7 +908,7 @@
       <c r="D20" s="3"/>
       <c r="G20" s="5">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -890,7 +917,7 @@
       <c r="D21" s="3"/>
       <c r="G21" s="5">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -899,7 +926,7 @@
       <c r="D22" s="3"/>
       <c r="G22" s="5">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -908,7 +935,7 @@
       <c r="D23" s="3"/>
       <c r="G23" s="5">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -921,7 +948,7 @@
       <c r="F24" s="20"/>
       <c r="G24" s="21">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="18"/>
@@ -939,15 +966,13 @@
       <c r="E25" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="3">
-        <v>5</v>
-      </c>
+      <c r="F25" s="3"/>
       <c r="G25" s="5">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H25" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I25" s="23" t="s">
         <v>30</v>
@@ -965,10 +990,10 @@
       </c>
       <c r="G26" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H26" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I26" s="23" t="s">
         <v>31</v>
@@ -977,7 +1002,7 @@
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G27" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H27" s="13"/>
       <c r="I27" s="9"/>
@@ -988,7 +1013,7 @@
       <c r="D28" s="3"/>
       <c r="G28" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H28" s="13"/>
       <c r="I28" s="9"/>
@@ -999,7 +1024,7 @@
       <c r="D29" s="3"/>
       <c r="G29" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H29" s="13"/>
       <c r="I29" s="9"/>
@@ -1012,7 +1037,7 @@
       <c r="F30" s="21"/>
       <c r="G30" s="21">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H30" s="20"/>
       <c r="I30" s="18"/>
@@ -1030,7 +1055,7 @@
       <c r="D31" s="3"/>
       <c r="G31" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H31" s="13"/>
       <c r="I31" s="9"/>
@@ -1041,7 +1066,7 @@
       <c r="D32" s="3"/>
       <c r="G32" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H32" s="13"/>
       <c r="I32" s="9"/>
@@ -1052,7 +1077,7 @@
       <c r="D33" s="3"/>
       <c r="G33" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H33" s="13"/>
       <c r="I33" s="9"/>
@@ -1063,7 +1088,7 @@
       <c r="D34" s="3"/>
       <c r="G34" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H34" s="13"/>
       <c r="I34" s="9"/>
@@ -1074,7 +1099,7 @@
       <c r="D35" s="3"/>
       <c r="G35" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H35" s="13"/>
       <c r="I35" s="9"/>
@@ -1087,7 +1112,7 @@
       <c r="F36" s="21"/>
       <c r="G36" s="21">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H36" s="20"/>
       <c r="I36" s="18"/>
@@ -1105,7 +1130,7 @@
       <c r="D37" s="3"/>
       <c r="G37" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H37" s="13"/>
       <c r="I37" s="9"/>
@@ -1116,7 +1141,7 @@
       <c r="D38" s="3"/>
       <c r="G38" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H38" s="13"/>
       <c r="I38" s="9"/>
@@ -1127,7 +1152,7 @@
       <c r="D39" s="3"/>
       <c r="G39" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="9"/>
@@ -1138,7 +1163,7 @@
       <c r="D40" s="3"/>
       <c r="G40" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H40" s="13"/>
       <c r="I40" s="9"/>
@@ -1149,7 +1174,7 @@
       <c r="D41" s="3"/>
       <c r="G41" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H41" s="13"/>
       <c r="I41" s="9"/>
@@ -1162,7 +1187,7 @@
       <c r="F42" s="21"/>
       <c r="G42" s="21">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H42" s="20"/>
       <c r="I42" s="18"/>
@@ -1180,7 +1205,7 @@
       <c r="D43" s="3"/>
       <c r="G43" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H43" s="13"/>
       <c r="I43" s="9"/>
@@ -1194,7 +1219,7 @@
       <c r="F44" s="13"/>
       <c r="G44" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="9"/>
@@ -1206,7 +1231,7 @@
       <c r="F45" s="13"/>
       <c r="G45" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H45" s="13"/>
       <c r="I45" s="9"/>
@@ -1220,7 +1245,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="9"/>
@@ -1232,7 +1257,7 @@
       <c r="F47" s="13"/>
       <c r="G47" s="5">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H47" s="13"/>
       <c r="I47" s="9"/>
@@ -1247,7 +1272,7 @@
       <c r="F48" s="20"/>
       <c r="G48" s="21">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H48" s="20"/>
       <c r="I48" s="18"/>

</xml_diff>

<commit_message>
Add STAT110 (Introduction to probability (2nd ed.))
</commit_message>
<xml_diff>
--- a/Administration/Training component.xlsx
+++ b/Administration/Training component.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\Administration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F743E1A-9390-49FB-AAFF-E561271D195C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15A6BE6-C097-41ED-BC25-076E1288DD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="6105" windowWidth="17070" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="2715" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
     <t>Johan's latent variable model</t>
   </si>
   <si>
-    <t>Under construction</t>
+    <t>Enrolled</t>
   </si>
 </sst>
 </file>
@@ -260,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -343,11 +343,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,10 +573,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:I999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -653,7 +659,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="5">
-        <f t="shared" ref="G3:G48" si="0">G2+F3</f>
+        <f t="shared" ref="G3:G47" si="0">G2+F3</f>
         <v>5</v>
       </c>
       <c r="H3" s="24" t="s">
@@ -681,70 +687,70 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="10" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="29">
+        <v>6</v>
+      </c>
+      <c r="G5" s="21">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="27"/>
+    </row>
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="F5" s="11">
+      <c r="H6" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="11">
         <v>2</v>
-      </c>
-      <c r="G5" s="5">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="16">
-        <v>6</v>
-      </c>
-      <c r="G6" s="21">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="H6" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="27"/>
-    </row>
-    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2022</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="3">
-        <v>3</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H7" s="25" t="s">
-        <v>36</v>
+      <c r="H7" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -759,7 +765,9 @@
     <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="5">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -775,55 +783,55 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="G11" s="5">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
+      <c r="H11" s="21"/>
+      <c r="I11" s="17"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21">
+      <c r="A12" s="6">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="7">
+        <v>8</v>
+      </c>
+      <c r="G12" s="5">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="H12" s="21"/>
-      <c r="I12" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>3</v>
-      </c>
-      <c r="B13" s="3">
-        <v>2022</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="7">
-        <v>8</v>
-      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
       <c r="G13" s="5">
         <f t="shared" si="0"/>
         <v>26</v>
-      </c>
-      <c r="H13" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -854,52 +862,52 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="G17" s="5">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
+      <c r="H17" s="21"/>
+      <c r="I17" s="17"/>
     </row>
     <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21">
+      <c r="A18" s="6">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="3">
+        <v>5</v>
+      </c>
+      <c r="G18" s="5">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="17"/>
+        <v>31</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
-        <v>4</v>
-      </c>
-      <c r="B19" s="3">
-        <v>2023</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="3">
-        <v>5</v>
-      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
       <c r="G19" s="5">
         <f t="shared" si="0"/>
         <v>31</v>
-      </c>
-      <c r="H19" s="25" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -930,76 +938,78 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="G23" s="5">
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
+      <c r="H23" s="20"/>
+      <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="21">
+      <c r="A24" s="6">
+        <v>5</v>
+      </c>
+      <c r="B24" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="5">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="H24" s="20"/>
-      <c r="I24" s="18"/>
+      <c r="H24" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="6">
-        <v>5</v>
-      </c>
-      <c r="B25" s="3">
-        <v>2023</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="3">
+        <v>3</v>
+      </c>
       <c r="G25" s="5">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H25" s="26" t="s">
         <v>35</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="3">
-        <v>3</v>
-      </c>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G26" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H26" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="I26" s="23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H26" s="13"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
       <c r="G27" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1019,39 +1029,39 @@
       <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="G29" s="5">
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H29" s="13"/>
-      <c r="I29" s="9"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="18"/>
     </row>
     <row r="30" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21">
+      <c r="A30" s="6">
+        <v>6</v>
+      </c>
+      <c r="B30" s="3">
+        <v>2024</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="G30" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H30" s="20"/>
-      <c r="I30" s="18"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="9"/>
     </row>
     <row r="31" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="6">
-        <v>6</v>
-      </c>
-      <c r="B31" s="3">
-        <v>2024</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="G31" s="5">
         <f t="shared" si="0"/>
@@ -1094,39 +1104,39 @@
       <c r="I34" s="9"/>
     </row>
     <row r="35" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="G35" s="5">
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="9"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="18"/>
     </row>
     <row r="36" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21">
+      <c r="A36" s="6">
+        <v>7</v>
+      </c>
+      <c r="B36" s="3">
+        <v>2024</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="G36" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H36" s="20"/>
-      <c r="I36" s="18"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="9"/>
     </row>
     <row r="37" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="6">
-        <v>7</v>
-      </c>
-      <c r="B37" s="3">
-        <v>2024</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="G37" s="5">
         <f t="shared" si="0"/>
@@ -1169,40 +1179,43 @@
       <c r="I40" s="9"/>
     </row>
     <row r="41" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="G41" s="5">
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H41" s="13"/>
-      <c r="I41" s="9"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="18"/>
     </row>
     <row r="42" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21">
+      <c r="A42" s="6">
+        <v>8</v>
+      </c>
+      <c r="B42" s="3">
+        <v>2025</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="G42" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H42" s="20"/>
-      <c r="I42" s="18"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="9"/>
     </row>
     <row r="43" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="6">
-        <v>8</v>
-      </c>
-      <c r="B43" s="3">
-        <v>2025</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" s="3"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" s="13"/>
       <c r="G43" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1211,11 +1224,9 @@
       <c r="I43" s="9"/>
     </row>
     <row r="44" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="12" t="s">
-        <v>24</v>
-      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
       <c r="F44" s="13"/>
       <c r="G44" s="5">
         <f t="shared" si="0"/>
@@ -1225,9 +1236,11 @@
       <c r="I44" s="9"/>
     </row>
     <row r="45" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B45" s="3"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="F45" s="13"/>
       <c r="G45" s="5">
         <f t="shared" si="0"/>
@@ -1237,11 +1250,9 @@
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="12" t="s">
-        <v>25</v>
-      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
       <c r="F46" s="13"/>
       <c r="G46" s="5">
         <f t="shared" si="0"/>
@@ -1251,31 +1262,24 @@
       <c r="I46" s="9"/>
     </row>
     <row r="47" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B47" s="3"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="5">
+      <c r="B47" s="17"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" s="20"/>
+      <c r="G47" s="21">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H47" s="13"/>
-      <c r="I47" s="9"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="18"/>
     </row>
     <row r="48" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B48" s="17"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F48" s="20"/>
-      <c r="G48" s="21">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="H48" s="20"/>
-      <c r="I48" s="18"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
     </row>
     <row r="49" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B49" s="3"/>
@@ -6032,11 +6036,6 @@
       <c r="C999" s="3"/>
       <c r="D999" s="3"/>
     </row>
-    <row r="1000" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B1000" s="3"/>
-      <c r="C1000" s="3"/>
-      <c r="D1000" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update training component planner
</commit_message>
<xml_diff>
--- a/Administration/Training component.xlsx
+++ b/Administration/Training component.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tctan/uio/pc/Dokumenter/PhD/Administration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC258CD-B10D-9641-A8BC-D34BF9DB4EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE15D5B-8BEB-2C45-B2E3-88F3C6B6249B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25020" yWindow="8060" windowWidth="24320" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Year</t>
   </si>
@@ -73,15 +77,6 @@
     <t>Started</t>
   </si>
   <si>
-    <t>ECON9106B</t>
-  </si>
-  <si>
-    <t>Advanced applied econometrics</t>
-  </si>
-  <si>
-    <t>Readings in educational fairness and equity</t>
-  </si>
-  <si>
     <t>UV9102A</t>
   </si>
   <si>
@@ -100,9 +95,6 @@
     <t>Exchange semester?</t>
   </si>
   <si>
-    <t>Conference presentations (x3)</t>
-  </si>
-  <si>
     <t>Final Reading</t>
   </si>
   <si>
@@ -115,18 +107,6 @@
     <t>Cumulative Credits</t>
   </si>
   <si>
-    <t>Seek additional info from Rolf. 2 credits?</t>
-  </si>
-  <si>
-    <t>Turn this into a DIY course. Down to 5 credits?</t>
-  </si>
-  <si>
-    <t>Verify with Rolf: is 5 credits feasible?</t>
-  </si>
-  <si>
-    <t>1 credit point for each presentation?</t>
-  </si>
-  <si>
     <t>Notes &amp; Questions</t>
   </si>
   <si>
@@ -136,23 +116,29 @@
     <t>Vår</t>
   </si>
   <si>
-    <t>Require confirmation</t>
-  </si>
-  <si>
-    <t>Standard enrollment</t>
-  </si>
-  <si>
     <t>Johan's latent variable model</t>
   </si>
   <si>
     <t>Kappeseminar</t>
+  </si>
+  <si>
+    <t>Panel Data/Econometrics</t>
+  </si>
+  <si>
+    <t>DRE 7006 (BI)</t>
+  </si>
+  <si>
+    <t>UV9121</t>
+  </si>
+  <si>
+    <t>Process data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -194,8 +180,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,26 +208,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor rgb="FFD9EAD3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor rgb="FFFCE5CD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF9900FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -260,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -280,31 +254,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -319,20 +278,29 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -554,8 +522,8 @@
   </sheetPr>
   <dimension ref="A1:I999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -589,13 +557,13 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -606,7 +574,7 @@
         <v>2021</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>6</v>
@@ -621,7 +589,7 @@
         <f>F2</f>
         <v>3</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -641,7 +609,7 @@
         <f t="shared" ref="G3:G47" si="0">G2+F3</f>
         <v>5</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -661,28 +629,28 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H4" s="19" t="s">
-        <v>10</v>
+      <c r="H4" s="21" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="17">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="12">
         <v>6</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="11">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="22"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="6">
@@ -692,13 +660,13 @@
         <v>2022</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F6" s="3">
         <v>3</v>
@@ -707,47 +675,36 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="10">
-        <v>2</v>
+      <c r="D7" s="18"/>
+      <c r="E7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>28</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0</v>
-      </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -758,7 +715,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="5">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -767,21 +724,21 @@
       <c r="D10" s="3"/>
       <c r="G10" s="5">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16">
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="14"/>
+        <v>16</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="6">
@@ -791,27 +748,17 @@
         <v>2022</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="7">
-        <v>8</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="5">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>29</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="H12" s="20"/>
+      <c r="I12" s="19"/>
     </row>
     <row r="13" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B13" s="3"/>
@@ -819,7 +766,7 @@
       <c r="D13" s="3"/>
       <c r="G13" s="5">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -828,7 +775,7 @@
       <c r="D14" s="3"/>
       <c r="G14" s="5">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -837,7 +784,7 @@
       <c r="D15" s="3"/>
       <c r="G15" s="5">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -846,21 +793,21 @@
       <c r="D16" s="3"/>
       <c r="G16" s="5">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="H17" s="16"/>
-      <c r="I17" s="14"/>
+        <v>16</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="6">
@@ -870,41 +817,63 @@
         <v>2023</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F18" s="3">
         <v>5</v>
       </c>
       <c r="G18" s="5">
         <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="5">
+        <v>6</v>
+      </c>
       <c r="G19" s="5">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="5">
+        <v>3</v>
+      </c>
       <c r="G20" s="5">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -913,7 +882,7 @@
       <c r="D21" s="3"/>
       <c r="G21" s="5">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -922,23 +891,23 @@
       <c r="D22" s="3"/>
       <c r="G22" s="5">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11">
         <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="14"/>
+        <v>30</v>
+      </c>
+      <c r="H23" s="11"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="6">
@@ -948,48 +917,36 @@
         <v>2023</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="5">
         <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="H24" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I24" s="18" t="s">
         <v>30</v>
       </c>
+      <c r="H24" s="15"/>
+      <c r="I24" s="13"/>
     </row>
     <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="3">
-        <v>3</v>
-      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="3"/>
       <c r="G25" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="H25" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>31</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H25" s="15"/>
+      <c r="I25" s="13"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G26" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -998,7 +955,7 @@
       <c r="D27" s="3"/>
       <c r="G27" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -1007,21 +964,21 @@
       <c r="D28" s="3"/>
       <c r="G28" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="H29" s="16"/>
-      <c r="I29" s="14"/>
+        <v>30</v>
+      </c>
+      <c r="H29" s="11"/>
+      <c r="I29" s="9"/>
     </row>
     <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="6">
@@ -1031,12 +988,12 @@
         <v>2024</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D30" s="3"/>
       <c r="G30" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -1045,7 +1002,7 @@
       <c r="D31" s="3"/>
       <c r="G31" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -1054,7 +1011,7 @@
       <c r="D32" s="3"/>
       <c r="G32" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -1063,7 +1020,7 @@
       <c r="D33" s="3"/>
       <c r="G33" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -1072,21 +1029,21 @@
       <c r="D34" s="3"/>
       <c r="G34" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16">
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="H35" s="16"/>
-      <c r="I35" s="14"/>
+        <v>30</v>
+      </c>
+      <c r="H35" s="11"/>
+      <c r="I35" s="9"/>
     </row>
     <row r="36" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="6">
@@ -1096,12 +1053,12 @@
         <v>2024</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D36" s="3"/>
       <c r="G36" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -1110,7 +1067,7 @@
       <c r="D37" s="3"/>
       <c r="G37" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -1119,7 +1076,7 @@
       <c r="D38" s="3"/>
       <c r="G38" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -1128,7 +1085,7 @@
       <c r="D39" s="3"/>
       <c r="G39" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -1137,21 +1094,21 @@
       <c r="D40" s="3"/>
       <c r="G40" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16">
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="H41" s="16"/>
-      <c r="I41" s="14"/>
+        <v>30</v>
+      </c>
+      <c r="H41" s="11"/>
+      <c r="I41" s="9"/>
     </row>
     <row r="42" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="6">
@@ -1161,21 +1118,21 @@
         <v>2025</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D42" s="3"/>
       <c r="G42" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="E43" s="11" t="s">
-        <v>24</v>
+      <c r="E43" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="G43" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -1184,16 +1141,16 @@
       <c r="D44" s="3"/>
       <c r="G44" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="E45" s="11" t="s">
-        <v>25</v>
+      <c r="E45" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="G45" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="13" x14ac:dyDescent="0.15">
@@ -1202,23 +1159,23 @@
       <c r="D46" s="3"/>
       <c r="G46" s="5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16">
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="H47" s="16"/>
-      <c r="I47" s="14"/>
+        <v>30</v>
+      </c>
+      <c r="H47" s="11"/>
+      <c r="I47" s="9"/>
     </row>
     <row r="48" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B48" s="3"/>

</xml_diff>